<commit_message>
fix engine type parameters
</commit_message>
<xml_diff>
--- a/dtv_backend/data/DTV_shiptypes_database.xlsx
+++ b/dtv_backend/data/DTV_shiptypes_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baart_f/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baart_f/src/digitaltwin-waterway/dtv_backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37BE802-5A39-6B48-B421-8A9AE14D24E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A954102-DF63-3746-B92D-EA2D3E197879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17000" yWindow="0" windowWidth="16600" windowHeight="21000" xr2:uid="{1ED1099D-4BC9-49B6-B1CA-AFE2C82F23A7}"/>
+    <workbookView xWindow="3620" yWindow="760" windowWidth="29980" windowHeight="19940" xr2:uid="{1ED1099D-4BC9-49B6-B1CA-AFE2C82F23A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="132">
   <si>
     <t>I</t>
   </si>
@@ -411,19 +411,22 @@
     <t>Vessel type</t>
   </si>
   <si>
-    <t xml:space="preserve">Engine power minumum [kW] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engine power maximum [kW] </t>
-  </si>
-  <si>
-    <t>Engine power averge [kW]</t>
-  </si>
-  <si>
     <t>Bow thruster maximum [kW]</t>
   </si>
   <si>
     <t>Bow thruster minimum [kW]</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>Engine power minumum [kW]</t>
+  </si>
+  <si>
+    <t>Engine power maximum [kW]</t>
+  </si>
+  <si>
+    <t>Engine power average [kW]</t>
   </si>
 </sst>
 </file>
@@ -796,33 +799,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA60D031-48D8-4F7A-9139-CD0C7ED9F83A}">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="46.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" hidden="1" customWidth="1"/>
-    <col min="7" max="9" width="23.5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="24.5" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="18" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="18.1640625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="24.83203125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="26.5" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="20" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="12" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" hidden="1" customWidth="1"/>
+    <col min="8" max="10" width="23.5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" hidden="1" customWidth="1"/>
+    <col min="12" max="14" width="24.5" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="18" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="18.1640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="24.83203125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="26.5" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -830,93 +834,96 @@
         <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>75</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5</v>
-      </c>
-      <c r="G2">
-        <v>4.1900000000000004</v>
       </c>
       <c r="H2">
         <v>4.1900000000000004</v>
@@ -925,10 +932,10 @@
         <v>4.1900000000000004</v>
       </c>
       <c r="J2">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="K2">
         <v>28</v>
-      </c>
-      <c r="K2">
-        <v>23</v>
       </c>
       <c r="L2">
         <v>23</v>
@@ -936,79 +943,82 @@
       <c r="M2">
         <v>23</v>
       </c>
-      <c r="O2">
+      <c r="N2">
+        <v>23</v>
+      </c>
+      <c r="P2">
         <v>2.06</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>1.2</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>118</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>112</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>84</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>5.04</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>5.0599999999999996</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5.09</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>39</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>38.619999999999997</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>38.89</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>39.53</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>2.5</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2.19</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>4.2699999999999996</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>312</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>367</v>
-      </c>
-      <c r="T3">
-        <v>175</v>
       </c>
       <c r="U3">
         <v>175</v>
@@ -1017,551 +1027,575 @@
         <v>175</v>
       </c>
       <c r="W3">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="X3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>72</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4">
         <v>6.6</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>5.77</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>6.6</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>6.64</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>55</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>41.98</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>50.32</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>61.62</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>2.6</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>2.31</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>5.13</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>490</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>577</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>240</v>
-      </c>
-      <c r="U4">
-        <v>300</v>
       </c>
       <c r="V4">
         <v>300</v>
       </c>
       <c r="W4">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="X4">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
       </c>
       <c r="E5" t="s">
         <v>50</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5">
         <v>7.2</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>7</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>7.2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>7.26</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>70</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>54.95</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>62.73</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>69.98</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>2.6</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>2.31</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>1</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>5.32</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>677</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>796</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>490</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>640</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>435</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>160</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>87</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>8.1999999999999993</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>7.47</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>8.19</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>8.2200000000000006</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>73</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>61.04</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>67</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>73</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>2.7</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>2.41</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>1.2</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>5.32</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>808</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>951</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>490</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>640</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>435</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>160</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>53</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>8.1999999999999993</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>8.18</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>8.1999999999999993</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>8.24</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>85</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>76.95</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>79.97</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>84.96</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>2.7</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>2.4</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>1.2</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>4.95</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>995</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>1171</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>490</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>640</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>435</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>160</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>9.5</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>8.94</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>9.42</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>9.5</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>85</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>73</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>80.069999999999993</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>85.5</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>2.9</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>2.57</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>1.2</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>5.4</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>1272</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>1497</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>750</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>1070</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>690</v>
-      </c>
-      <c r="W8">
-        <v>250</v>
       </c>
       <c r="X8">
         <v>250</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="Y8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>9.5</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>9</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>9.5</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>9.5299999999999994</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>105</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>90</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>100.18</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>109.75</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>3</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>2.65</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>1.2</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>5.59</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>1722</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>2026</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>750</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>1070</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>690</v>
-      </c>
-      <c r="W9">
-        <v>250</v>
       </c>
       <c r="X9">
         <v>250</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="Y9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>11.4</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>10.6</v>
-      </c>
-      <c r="H10">
-        <v>11.45</v>
       </c>
       <c r="I10">
         <v>11.45</v>
       </c>
       <c r="J10">
+        <v>11.45</v>
+      </c>
+      <c r="K10">
         <v>110</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>93</v>
-      </c>
-      <c r="L10">
-        <v>110</v>
       </c>
       <c r="M10">
         <v>110</v>
       </c>
       <c r="N10">
+        <v>110</v>
+      </c>
+      <c r="O10">
         <v>3.5</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>3.14</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>1.4</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>6.21</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>2286</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>2689</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>1375</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>1750</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>1425</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>435</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>705</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>11.4</v>
-      </c>
-      <c r="G11">
-        <v>11.45</v>
       </c>
       <c r="H11">
         <v>11.45</v>
@@ -1570,158 +1604,164 @@
         <v>11.45</v>
       </c>
       <c r="J11">
+        <v>11.45</v>
+      </c>
+      <c r="K11">
         <v>135</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>125</v>
-      </c>
-      <c r="L11">
-        <v>135</v>
       </c>
       <c r="M11">
         <v>135</v>
       </c>
       <c r="N11">
+        <v>135</v>
+      </c>
+      <c r="O11">
         <v>3.5</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>3.08</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>1.4</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>6.36</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>3315</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>3900</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>1375</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>1750</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>1425</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>435</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>705</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>72</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>13.6</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>13.32</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>13.5</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>14.13</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>110</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>97</v>
-      </c>
-      <c r="L12">
-        <v>110</v>
       </c>
       <c r="M12">
         <v>110</v>
       </c>
       <c r="N12">
+        <v>110</v>
+      </c>
+      <c r="O12">
         <v>4</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>3.56</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>1.6</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>7.18</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>3342</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>3932</v>
-      </c>
-      <c r="T12">
-        <v>2400</v>
       </c>
       <c r="U12">
         <v>2400</v>
       </c>
       <c r="V12">
+        <v>2400</v>
+      </c>
+      <c r="W12">
         <v>2015</v>
-      </c>
-      <c r="W12">
-        <v>1135</v>
       </c>
       <c r="X12">
         <v>1135</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="Y12">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>72</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>14.2</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>13.34</v>
-      </c>
-      <c r="H13">
-        <v>14.2</v>
       </c>
       <c r="I13">
         <v>14.2</v>
       </c>
       <c r="J13">
+        <v>14.2</v>
+      </c>
+      <c r="K13">
         <v>185</v>
-      </c>
-      <c r="K13">
-        <v>135</v>
       </c>
       <c r="L13">
         <v>135</v>
@@ -1730,69 +1770,72 @@
         <v>135</v>
       </c>
       <c r="N13">
+        <v>135</v>
+      </c>
+      <c r="O13">
         <v>4</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>3.55</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>1.6</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>7.29</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>4408</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>5186</v>
-      </c>
-      <c r="T13">
-        <v>2400</v>
       </c>
       <c r="U13">
         <v>2400</v>
       </c>
       <c r="V13">
+        <v>2400</v>
+      </c>
+      <c r="W13">
         <v>2015</v>
-      </c>
-      <c r="W13">
-        <v>1135</v>
       </c>
       <c r="X13">
         <v>1135</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y13">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>72</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>60</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>102</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>17</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>15</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>16.84</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>17.39</v>
-      </c>
-      <c r="J14">
-        <v>135</v>
       </c>
       <c r="K14">
         <v>135</v>
@@ -1804,99 +1847,102 @@
         <v>135</v>
       </c>
       <c r="N14">
+        <v>135</v>
+      </c>
+      <c r="O14">
         <v>4</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>3.57</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>1.6</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>8.3699999999999992</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>5015</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>5900</v>
-      </c>
-      <c r="T14">
-        <v>2400</v>
       </c>
       <c r="U14">
         <v>2400</v>
       </c>
       <c r="V14">
+        <v>2400</v>
+      </c>
+      <c r="W14">
         <v>2015</v>
-      </c>
-      <c r="W14">
-        <v>1135</v>
       </c>
       <c r="X14">
         <v>1135</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y14">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>2</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>86</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>10.1</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>10.09</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>10.1</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>10.5</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>38.5</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>39</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>40</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>59</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>2.5</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>2.19</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>1</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>4.2699999999999996</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>629</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>740</v>
-      </c>
-      <c r="T15">
-        <v>175</v>
       </c>
       <c r="U15">
         <v>175</v>
@@ -1905,72 +1951,75 @@
         <v>175</v>
       </c>
       <c r="W15">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="X15">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>73</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>4</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>85</v>
-      </c>
-      <c r="F16">
-        <v>5.05</v>
       </c>
       <c r="G16">
         <v>5.05</v>
       </c>
       <c r="H16">
+        <v>5.05</v>
+      </c>
+      <c r="I16">
         <v>5.07</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>80</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>78</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>79</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>80</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>2.5</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>2.1800000000000002</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>1</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>4.2699999999999996</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>647</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>761</v>
-      </c>
-      <c r="T16">
-        <v>175</v>
       </c>
       <c r="U16">
         <v>175</v>
@@ -1979,412 +2028,430 @@
         <v>175</v>
       </c>
       <c r="W16">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="X16">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
         <v>73</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>92</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>9.5</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>8.2200000000000006</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>9.5</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>9.5399999999999991</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>180</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>117</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>165</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>185</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>3</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>2.81</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>1.2</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>5.4</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>1535</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>1806</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>750</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>1070</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>690</v>
-      </c>
-      <c r="W17">
-        <v>250</v>
       </c>
       <c r="X17">
         <v>250</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>98</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>11.4</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>11</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>11.4</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>11.45</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>180</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>171</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>180</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>187</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>3.5</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>3.57</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>1.5</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>6.5</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>4451</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>5236</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
         <v>73</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>100</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>18.5</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>15.24</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>18.54</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>19</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>103</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>67</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>85</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>105</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>3</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>2.76</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>1.2</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>5.4</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>1921</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>2260</v>
-      </c>
-      <c r="T19">
-        <v>2400</v>
       </c>
       <c r="U19">
         <v>2400</v>
       </c>
       <c r="V19">
+        <v>2400</v>
+      </c>
+      <c r="W19">
         <v>2015</v>
-      </c>
-      <c r="W19">
-        <v>1135</v>
       </c>
       <c r="X19">
         <v>1135</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y19">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>15</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>101</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>22.8</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>20.9</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>22.8</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>23.4</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>105</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>95</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>108</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>110</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>3.5</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>3.63</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>1.5</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>6.5</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>4636</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>5454</v>
-      </c>
-      <c r="T20">
-        <v>2400</v>
       </c>
       <c r="U20">
         <v>2400</v>
       </c>
       <c r="V20">
+        <v>2400</v>
+      </c>
+      <c r="W20">
         <v>2015</v>
-      </c>
-      <c r="W20">
-        <v>1135</v>
       </c>
       <c r="X20">
         <v>1135</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y20">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>18</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>104</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>22.8</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>21</v>
-      </c>
-      <c r="H21">
-        <v>22.8</v>
       </c>
       <c r="I21">
         <v>22.8</v>
       </c>
       <c r="J21">
+        <v>22.8</v>
+      </c>
+      <c r="K21">
         <v>185</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>172</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>184</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>187</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>3.5</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>3.68</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>1.5</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>6.5</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <v>6923</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>8145</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
         <v>74</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>19</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>77</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>5.2</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>4.7699999999999996</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>5.13</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>5.15</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>55</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>43</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>55</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>56</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>1.9</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>1.84</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>1.5</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>6.02</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>85</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>100</v>
-      </c>
-      <c r="T22">
-        <v>175</v>
       </c>
       <c r="U22">
         <v>175</v>
@@ -2393,500 +2460,524 @@
         <v>175</v>
       </c>
       <c r="W22">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="X22">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>78</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
         <v>74</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>19</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>79</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>6.7</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>5.94</v>
-      </c>
-      <c r="H23">
-        <v>6.66</v>
       </c>
       <c r="I23">
         <v>6.66</v>
       </c>
       <c r="J23">
+        <v>6.66</v>
+      </c>
+      <c r="K23">
         <v>61</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>46</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>61</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>71</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>2.6</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>2.4300000000000002</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>1.65</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>6.02</v>
       </c>
-      <c r="R23">
+      <c r="S23">
         <v>357</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <v>420</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>240</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>300</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>250</v>
-      </c>
-      <c r="W23">
-        <v>130</v>
       </c>
       <c r="X23">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y23">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>80</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
         <v>74</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>19</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>81</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>7.5</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>7.23</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>7.46</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>7.5</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>78</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>61</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>78</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>85</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>2.6</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>2.42</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>2</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>6.02</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <v>544</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <v>640</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>82</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
         <v>74</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>19</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>83</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>8.1999999999999993</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>7.77</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>8.18</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>8.36</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>85</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>55</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>84</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>88</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>2.7</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>2.4700000000000002</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>2</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>6.02</v>
       </c>
-      <c r="R25">
+      <c r="S25">
         <v>804</v>
       </c>
-      <c r="S25">
+      <c r="T25">
         <v>946</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>490</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <v>640</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>435</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>160</v>
       </c>
-      <c r="X25">
+      <c r="Y25">
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
         <v>74</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>25</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>91</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>9.5</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>9.4499999999999993</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>9.5</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>9.5299999999999994</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>94</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>85</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>94</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>104</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>3</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>2.72</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>2.06</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>6.02</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <v>1256</v>
       </c>
-      <c r="S26">
+      <c r="T26">
         <v>1478</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <v>1070</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>690</v>
-      </c>
-      <c r="W26">
-        <v>250</v>
       </c>
       <c r="X26">
         <v>250</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y26">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>94</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
         <v>74</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>27</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>95</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>11.4</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>11.2</v>
-      </c>
-      <c r="H27">
-        <v>11.4</v>
       </c>
       <c r="I27">
         <v>11.4</v>
       </c>
       <c r="J27">
+        <v>11.4</v>
+      </c>
+      <c r="K27">
         <v>92</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>95</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>102</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>107</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>3.5</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>3.18</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>2.1</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>6.02</v>
       </c>
-      <c r="R27">
+      <c r="S27">
         <v>1893</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <v>2227</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>1375</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>1750</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>1425</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>435</v>
       </c>
-      <c r="X27">
+      <c r="Y27">
         <v>705</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
         <v>74</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>29</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>124</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>11.4</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>11.2</v>
-      </c>
-      <c r="H28">
-        <v>11.4</v>
       </c>
       <c r="I28">
         <v>11.4</v>
       </c>
       <c r="J28">
+        <v>11.4</v>
+      </c>
+      <c r="K28">
         <v>110</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>3.5</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>3.18</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>2.1</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>6.02</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>1375</v>
       </c>
-      <c r="U28">
+      <c r="V28">
         <v>1750</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>1425</v>
       </c>
-      <c r="W28">
+      <c r="X28">
         <v>435</v>
       </c>
-      <c r="X28">
+      <c r="Y28">
         <v>705</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
         <v>74</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>31</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>107</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>11.4</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>11.2</v>
-      </c>
-      <c r="H29">
-        <v>11.4</v>
       </c>
       <c r="I29">
         <v>11.4</v>
       </c>
       <c r="J29">
+        <v>11.4</v>
+      </c>
+      <c r="K29">
         <v>136</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>3.5</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>3.18</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <v>2.1</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>6.02</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>1375</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>1750</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>1425</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>435</v>
       </c>
-      <c r="X29">
+      <c r="Y29">
         <v>705</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
         <v>74</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>37</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>97</v>
-      </c>
-      <c r="F30">
-        <v>11.4</v>
       </c>
       <c r="G30">
         <v>11.4</v>
@@ -2898,128 +2989,134 @@
         <v>11.4</v>
       </c>
       <c r="J30">
+        <v>11.4</v>
+      </c>
+      <c r="K30">
         <v>185</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>171</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>178</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>190</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>4</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>3.05</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <v>2.16</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>6.93</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <v>4671</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <v>5495</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
         <v>74</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>33</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>99</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>22.8</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>22.77</v>
-      </c>
-      <c r="H31">
-        <v>22.8</v>
       </c>
       <c r="I31">
         <v>22.8</v>
       </c>
       <c r="J31">
+        <v>22.8</v>
+      </c>
+      <c r="K31">
         <v>105</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>98</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>110</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>135</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>4</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>3.13</v>
       </c>
-      <c r="P31">
+      <c r="Q31">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>6.93</v>
       </c>
-      <c r="R31">
+      <c r="S31">
         <v>4761</v>
       </c>
-      <c r="S31">
+      <c r="T31">
         <v>5601</v>
-      </c>
-      <c r="T31">
-        <v>2400</v>
       </c>
       <c r="U31">
         <v>2400</v>
       </c>
       <c r="V31">
+        <v>2400</v>
+      </c>
+      <c r="W31">
         <v>2015</v>
-      </c>
-      <c r="W31">
-        <v>1135</v>
       </c>
       <c r="X31">
         <v>1135</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y31">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
         <v>74</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>35</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>103</v>
-      </c>
-      <c r="F32">
-        <v>22.8</v>
       </c>
       <c r="G32">
         <v>22.8</v>
@@ -3031,151 +3128,160 @@
         <v>22.8</v>
       </c>
       <c r="J32">
+        <v>22.8</v>
+      </c>
+      <c r="K32">
         <v>193</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>185</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>189</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>193</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>4</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>3.57</v>
       </c>
-      <c r="P32">
+      <c r="Q32">
         <v>1.8</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>9.35</v>
       </c>
-      <c r="R32">
+      <c r="S32">
         <v>9508</v>
       </c>
-      <c r="S32">
+      <c r="T32">
         <v>11186</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
       <c r="B33" t="s">
         <v>39</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
         <v>74</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>40</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>106</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>34.200000000000003</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>33.200000000000003</v>
-      </c>
-      <c r="H33">
-        <v>34.200000000000003</v>
       </c>
       <c r="I33">
         <v>34.200000000000003</v>
       </c>
       <c r="J33">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="K33">
         <v>195</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>185</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>193</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>194</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>4</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>3.58</v>
       </c>
-      <c r="P33">
+      <c r="Q33">
         <v>1.7</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
         <v>9.35</v>
       </c>
-      <c r="R33">
+      <c r="S33">
         <v>14019</v>
       </c>
-      <c r="S33">
+      <c r="T33">
         <v>16493</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
       <c r="B34" t="s">
         <v>42</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
         <v>74</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>43</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>105</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>22.8</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>22.78</v>
-      </c>
-      <c r="H34">
-        <v>22.8</v>
       </c>
       <c r="I34">
         <v>22.8</v>
       </c>
       <c r="J34">
+        <v>22.8</v>
+      </c>
+      <c r="K34">
         <v>270</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>231</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>268</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>275</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <v>4</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>3.54</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>1.8</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>9.35</v>
       </c>
-      <c r="R34">
+      <c r="S34">
         <v>14243</v>
       </c>
-      <c r="S34">
+      <c r="T34">
         <v>16757</v>
       </c>
     </row>

</xml_diff>